<commit_message>
Add new data sheets from new weather station, water potential, and porometer values.
</commit_message>
<xml_diff>
--- a/data/dbg_cottonwood_plant trait summary_03.xlsx
+++ b/data/dbg_cottonwood_plant trait summary_03.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinpannikkat/Documents/schoolwork/FEL/garisom/03_test_data/fremont-poplar-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CEEB42-D00C-A240-9178-715685DC95D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0AF7CA-5150-8743-8FE2-A2D41EC83D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Repeated measurements" sheetId="1" r:id="rId1"/>
@@ -2143,8 +2143,8 @@
   </sheetPr>
   <dimension ref="A1:AB788"/>
   <sheetViews>
-    <sheetView topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="I184" sqref="I184:I198"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -78083,6 +78083,7 @@
     <mergeCell ref="N1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -78093,8 +78094,8 @@
   </sheetPr>
   <dimension ref="A1:Z736"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="N79" sqref="N79"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K90" sqref="K90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add weibull params to plant trait sheet.
</commit_message>
<xml_diff>
--- a/data/dbg_cottonwood_plant trait summary_03.xlsx
+++ b/data/dbg_cottonwood_plant trait summary_03.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinpannikkat/Documents/schoolwork/FEL/garisom/03_test_data/fremont-poplar-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0AF7CA-5150-8743-8FE2-A2D41EC83D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696BAFB2-6EBD-C442-AF7D-86F921FB7168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="880" windowWidth="41120" windowHeight="25700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Repeated measurements" sheetId="1" r:id="rId1"/>
     <sheet name="One time measurements" sheetId="2" r:id="rId2"/>
-    <sheet name="Stem hydraulics" sheetId="3" r:id="rId3"/>
+    <sheet name="weibull" sheetId="5" r:id="rId3"/>
+    <sheet name="Stem hydraulics" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2615" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2632" uniqueCount="127">
   <si>
     <t>hydraulics</t>
   </si>
@@ -1617,6 +1618,45 @@
   <si>
     <t>Jmax</t>
   </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>estimate_P12</t>
+  </si>
+  <si>
+    <t>estimate_P50</t>
+  </si>
+  <si>
+    <t>conf.low_P12</t>
+  </si>
+  <si>
+    <t>conf.low_P50</t>
+  </si>
+  <si>
+    <t>conf.high_P12</t>
+  </si>
+  <si>
+    <t>conf.high_P50</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>conf.low_c</t>
+  </si>
+  <si>
+    <t>conf.low_b</t>
+  </si>
+  <si>
+    <t>conf.high_c</t>
+  </si>
+  <si>
+    <t>conf.high_b</t>
+  </si>
 </sst>
 </file>
 
@@ -1633,7 +1673,7 @@
     <numFmt numFmtId="171" formatCode="#,##0.0000000000"/>
     <numFmt numFmtId="172" formatCode="#,##0.00000000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1681,6 +1721,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1709,7 +1754,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1834,6 +1879,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2143,7 +2192,7 @@
   </sheetPr>
   <dimension ref="A1:AB788"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -78094,8 +78143,8 @@
   </sheetPr>
   <dimension ref="A1:Z736"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K90" sqref="K90"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="I90" sqref="I90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -84162,7 +84211,7 @@
         <f>AVERAGE(G37:G51)</f>
         <v>1.6186666666666667</v>
       </c>
-      <c r="F77" s="5">
+      <c r="F77" s="53">
         <f>C77/AVERAGE(I37:I51)</f>
         <v>1077.9887375589315</v>
       </c>
@@ -84221,7 +84270,7 @@
         <f>AVERAGE(G54:G68)</f>
         <v>1.7013333333333334</v>
       </c>
-      <c r="F78" s="5">
+      <c r="F78" s="53">
         <f>C78/AVERAGE(I54:I68)</f>
         <v>1063.6873707787734</v>
       </c>
@@ -85741,6 +85790,237 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9EB1CD-8FA1-7548-9530-3FCC02CBF0AC}">
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="K1" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="L1" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="M1" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+    </row>
+    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="52">
+        <v>2.21879692</v>
+      </c>
+      <c r="C2" s="52">
+        <v>2.5709419900000001</v>
+      </c>
+      <c r="D2" s="52">
+        <v>2.0822660499999999</v>
+      </c>
+      <c r="E2" s="52">
+        <v>2.43090042</v>
+      </c>
+      <c r="F2" s="52">
+        <v>2.3633450200000001</v>
+      </c>
+      <c r="G2" s="52">
+        <v>2.7109625899999998</v>
+      </c>
+      <c r="H2" s="52">
+        <v>11.4761141</v>
+      </c>
+      <c r="I2" s="52">
+        <v>2.6543754399999999</v>
+      </c>
+      <c r="J2" s="52">
+        <v>10.920286300000001</v>
+      </c>
+      <c r="K2" s="52">
+        <v>2.5138722800000002</v>
+      </c>
+      <c r="L2" s="52">
+        <v>12.319221900000001</v>
+      </c>
+      <c r="M2" s="52">
+        <v>2.79282904</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="52">
+        <v>2.28014231</v>
+      </c>
+      <c r="C3" s="52">
+        <v>2.6333419899999999</v>
+      </c>
+      <c r="D3" s="52">
+        <v>2.12760046</v>
+      </c>
+      <c r="E3" s="52">
+        <v>2.4818098599999998</v>
+      </c>
+      <c r="F3" s="52">
+        <v>2.4363307600000002</v>
+      </c>
+      <c r="G3" s="52">
+        <v>2.7918230999999998</v>
+      </c>
+      <c r="H3" s="52">
+        <v>11.7383892</v>
+      </c>
+      <c r="I3" s="52">
+        <v>2.7168610900000001</v>
+      </c>
+      <c r="J3" s="52">
+        <v>10.9778477</v>
+      </c>
+      <c r="K3" s="52">
+        <v>2.5660677399999998</v>
+      </c>
+      <c r="L3" s="52">
+        <v>12.411847</v>
+      </c>
+      <c r="M3" s="52">
+        <v>2.8754929100000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="52">
+        <v>2.3076028000000002</v>
+      </c>
+      <c r="C4" s="52">
+        <v>2.6608802900000001</v>
+      </c>
+      <c r="D4" s="52">
+        <v>2.1627233600000002</v>
+      </c>
+      <c r="E4" s="52">
+        <v>2.5162265800000001</v>
+      </c>
+      <c r="F4" s="52">
+        <v>2.45379214</v>
+      </c>
+      <c r="G4" s="52">
+        <v>2.8094894799999999</v>
+      </c>
+      <c r="H4" s="52">
+        <v>11.8676116</v>
+      </c>
+      <c r="I4" s="52">
+        <v>2.7443396</v>
+      </c>
+      <c r="J4" s="52">
+        <v>11.1664625</v>
+      </c>
+      <c r="K4" s="52">
+        <v>2.6001861599999998</v>
+      </c>
+      <c r="L4" s="52">
+        <v>12.4882756</v>
+      </c>
+      <c r="M4" s="52">
+        <v>2.89316584</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="52">
+        <v>2.3715587299999998</v>
+      </c>
+      <c r="C5" s="52">
+        <v>2.72552715</v>
+      </c>
+      <c r="D5" s="52">
+        <v>2.2012471900000001</v>
+      </c>
+      <c r="E5" s="52">
+        <v>2.5540011900000001</v>
+      </c>
+      <c r="F5" s="52">
+        <v>2.54166034</v>
+      </c>
+      <c r="G5" s="52">
+        <v>2.8953680500000001</v>
+      </c>
+      <c r="H5" s="52">
+        <v>12.1519724</v>
+      </c>
+      <c r="I5" s="52">
+        <v>2.8089833899999999</v>
+      </c>
+      <c r="J5" s="52">
+        <v>11.3734357</v>
+      </c>
+      <c r="K5" s="52">
+        <v>2.6376452499999998</v>
+      </c>
+      <c r="L5" s="52">
+        <v>12.9745481</v>
+      </c>
+      <c r="M5" s="52">
+        <v>2.9783243499999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>

</xml_diff>